<commit_message>
week 05 slides and many small things
</commit_message>
<xml_diff>
--- a/Raw Data/SNA/30ffm1rn_jp.xlsx
+++ b/Raw Data/SNA/30ffm1rn_jp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\co882078\Desktop\一時作業用\30推計\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1684bc3b7bd79ed3/_Teaching/_Course/MaD/Raw Data/SNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_D89F13B857BD77CFA9BC79F71B6FEEAB0EEFEE7B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36E22291-B0E6-784C-8D98-E7DF016CBE53}"/>
   <bookViews>
-    <workbookView xWindow="4176" yWindow="-12" windowWidth="28836" windowHeight="6372"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="33300" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="実数" sheetId="1" r:id="rId1"/>
@@ -17,11 +18,21 @@
     <sheet name="寄与度" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">増加率!$A:$A</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">実数!$A:$A</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">寄与度!$A:$A</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">実数!$A:$A</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">増加率!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -517,13 +528,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="#,##0.0;\-#,##0.0"/>
-    <numFmt numFmtId="178" formatCode="\-0.0"/>
-    <numFmt numFmtId="204" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0;\-#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="\-0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="14"/>
       <name val="ＭＳ 明朝"/>
@@ -532,12 +543,6 @@
     </font>
     <font>
       <sz val="7"/>
-      <name val="ＭＳ 明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <name val="ＭＳ 明朝"/>
       <family val="1"/>
       <charset val="128"/>
@@ -682,22 +687,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -738,39 +743,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -854,7 +859,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -929,6 +934,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -964,6 +986,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1139,25 +1178,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="72.6640625" style="3" customWidth="1"/>
-    <col min="2" max="26" width="15.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="72.7109375" style="3" customWidth="1"/>
+    <col min="2" max="26" width="15.7109375" style="3" customWidth="1"/>
     <col min="27" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="5" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -1174,7 +1215,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" customFormat="1">
       <c r="A5" s="22"/>
       <c r="B5" s="16" t="s">
         <v>1</v>
@@ -1252,7 +1293,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" customFormat="1">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -1282,7 +1323,7 @@
       <c r="Y6" s="18"/>
       <c r="Z6" s="19"/>
     </row>
-    <row r="7" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" customFormat="1">
       <c r="A7" s="24"/>
       <c r="B7" s="20">
         <v>1994</v>
@@ -1360,7 +1401,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" customFormat="1">
       <c r="A8" s="25" t="s">
         <v>12</v>
       </c>
@@ -1440,7 +1481,7 @@
         <v>299046.8</v>
       </c>
     </row>
-    <row r="9" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" customFormat="1">
       <c r="A9" s="23" t="s">
         <v>13</v>
       </c>
@@ -1520,7 +1561,7 @@
         <v>291331.3</v>
       </c>
     </row>
-    <row r="10" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" customFormat="1">
       <c r="A10" s="23" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1641,7 @@
         <v>294213.90000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" customFormat="1">
       <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
@@ -1680,7 +1721,7 @@
         <v>1287.7</v>
       </c>
     </row>
-    <row r="12" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" customFormat="1">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
@@ -1760,7 +1801,7 @@
         <v>4058.1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" customFormat="1">
       <c r="A13" s="23" t="s">
         <v>17</v>
       </c>
@@ -1790,7 +1831,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="36"/>
     </row>
-    <row r="14" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" customFormat="1">
       <c r="A14" s="23" t="s">
         <v>18</v>
       </c>
@@ -1870,7 +1911,7 @@
         <v>237402.5</v>
       </c>
     </row>
-    <row r="15" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" customFormat="1">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
@@ -1950,7 +1991,7 @@
         <v>54111.5</v>
       </c>
     </row>
-    <row r="16" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" customFormat="1">
       <c r="A16" s="23" t="s">
         <v>20</v>
       </c>
@@ -2030,7 +2071,7 @@
         <v>7723.3</v>
       </c>
     </row>
-    <row r="17" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" customFormat="1">
       <c r="A17" s="23"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2058,7 +2099,7 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="36"/>
     </row>
-    <row r="18" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" customFormat="1">
       <c r="A18" s="23" t="s">
         <v>21</v>
       </c>
@@ -2138,7 +2179,7 @@
         <v>107252.2</v>
       </c>
     </row>
-    <row r="19" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" customFormat="1">
       <c r="A19" s="23" t="s">
         <v>22</v>
       </c>
@@ -2168,7 +2209,7 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="36"/>
     </row>
-    <row r="20" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" customFormat="1">
       <c r="A20" s="23" t="s">
         <v>23</v>
       </c>
@@ -2248,7 +2289,7 @@
         <v>365323.4</v>
       </c>
     </row>
-    <row r="21" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" customFormat="1">
       <c r="A21" s="23" t="s">
         <v>24</v>
       </c>
@@ -2328,7 +2369,7 @@
         <v>40948.6</v>
       </c>
     </row>
-    <row r="22" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" customFormat="1">
       <c r="A22" s="23" t="s">
         <v>78</v>
       </c>
@@ -2408,7 +2449,7 @@
         <v>128394.5</v>
       </c>
     </row>
-    <row r="23" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" customFormat="1">
       <c r="A23" s="23" t="s">
         <v>25</v>
       </c>
@@ -2488,7 +2529,7 @@
         <v>126869.2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" customFormat="1">
       <c r="A24" s="23" t="s">
         <v>26</v>
       </c>
@@ -2568,7 +2609,7 @@
         <v>100798</v>
       </c>
     </row>
-    <row r="25" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" customFormat="1">
       <c r="A25" s="23" t="s">
         <v>27</v>
       </c>
@@ -2648,7 +2689,7 @@
         <v>15143</v>
       </c>
     </row>
-    <row r="26" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" customFormat="1">
       <c r="A26" s="23" t="s">
         <v>28</v>
       </c>
@@ -2728,7 +2769,7 @@
         <v>85741</v>
       </c>
     </row>
-    <row r="27" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" customFormat="1">
       <c r="A27" s="23" t="s">
         <v>29</v>
       </c>
@@ -2808,7 +2849,7 @@
         <v>26103.3</v>
       </c>
     </row>
-    <row r="28" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" customFormat="1">
       <c r="A28" s="23" t="s">
         <v>30</v>
       </c>
@@ -2888,7 +2929,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="29" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" customFormat="1">
       <c r="A29" s="35" t="s">
         <v>31</v>
       </c>
@@ -2968,7 +3009,7 @@
         <v>6582.2</v>
       </c>
     </row>
-    <row r="30" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" customFormat="1">
       <c r="A30" s="35" t="s">
         <v>32</v>
       </c>
@@ -3048,7 +3089,7 @@
         <v>18951.099999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" customFormat="1">
       <c r="A31" s="35" t="s">
         <v>95</v>
       </c>
@@ -3128,7 +3169,7 @@
         <v>1542.6</v>
       </c>
     </row>
-    <row r="32" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" customFormat="1">
       <c r="A32" s="35" t="s">
         <v>56</v>
       </c>
@@ -3208,7 +3249,7 @@
         <v>1477.3</v>
       </c>
     </row>
-    <row r="33" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" customFormat="1">
       <c r="A33" s="35" t="s">
         <v>96</v>
       </c>
@@ -3288,7 +3329,7 @@
         <v>225.1</v>
       </c>
     </row>
-    <row r="34" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" customFormat="1">
       <c r="A34" s="35" t="s">
         <v>97</v>
       </c>
@@ -3368,7 +3409,7 @@
         <v>479.3</v>
       </c>
     </row>
-    <row r="35" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" customFormat="1">
       <c r="A35" s="35" t="s">
         <v>98</v>
       </c>
@@ -3448,7 +3489,7 @@
         <v>204.9</v>
       </c>
     </row>
-    <row r="36" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" customFormat="1">
       <c r="A36" s="35" t="s">
         <v>99</v>
       </c>
@@ -3528,7 +3569,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="37" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" customFormat="1">
       <c r="A37" s="35" t="s">
         <v>29</v>
       </c>
@@ -3608,7 +3649,7 @@
         <v>39.1</v>
       </c>
     </row>
-    <row r="38" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" customFormat="1">
       <c r="A38" s="35" t="s">
         <v>33</v>
       </c>
@@ -3688,7 +3729,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="39" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" customFormat="1">
       <c r="A39" s="35" t="s">
         <v>34</v>
       </c>
@@ -3768,7 +3809,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="40" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" customFormat="1">
       <c r="A40" s="23" t="s">
         <v>35</v>
       </c>
@@ -3848,7 +3889,7 @@
         <v>-1745.3</v>
       </c>
     </row>
-    <row r="41" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" customFormat="1">
       <c r="A41" s="23" t="s">
         <v>36</v>
       </c>
@@ -3928,7 +3969,7 @@
         <v>92873</v>
       </c>
     </row>
-    <row r="42" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" customFormat="1">
       <c r="A42" s="23" t="s">
         <v>84</v>
       </c>
@@ -4008,7 +4049,7 @@
         <v>74618</v>
       </c>
     </row>
-    <row r="43" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" customFormat="1">
       <c r="A43" s="23" t="s">
         <v>85</v>
       </c>
@@ -4088,7 +4129,7 @@
         <v>18173.099999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" customFormat="1">
       <c r="A44" s="23" t="s">
         <v>37</v>
       </c>
@@ -4168,7 +4209,7 @@
         <v>94618.3</v>
       </c>
     </row>
-    <row r="45" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" customFormat="1">
       <c r="A45" s="23" t="s">
         <v>86</v>
       </c>
@@ -4248,7 +4289,7 @@
         <v>76935.5</v>
       </c>
     </row>
-    <row r="46" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" customFormat="1">
       <c r="A46" s="23" t="s">
         <v>87</v>
       </c>
@@ -4328,7 +4369,7 @@
         <v>17869.900000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" customFormat="1">
       <c r="A47" s="23" t="s">
         <v>38</v>
       </c>
@@ -4358,7 +4399,7 @@
       <c r="Y47" s="6"/>
       <c r="Z47" s="36"/>
     </row>
-    <row r="48" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" customFormat="1">
       <c r="A48" s="23" t="s">
         <v>72</v>
       </c>
@@ -4438,7 +4479,7 @@
         <v>533667.9</v>
       </c>
     </row>
-    <row r="49" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" customFormat="1">
       <c r="A49" s="23"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -4466,7 +4507,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="36"/>
     </row>
-    <row r="50" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" customFormat="1">
       <c r="A50" s="23" t="s">
         <v>39</v>
       </c>
@@ -4546,7 +4587,7 @@
         <v>610.4</v>
       </c>
     </row>
-    <row r="51" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" customFormat="1">
       <c r="A51" s="23"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -4574,7 +4615,7 @@
       <c r="Y51" s="6"/>
       <c r="Z51" s="36"/>
     </row>
-    <row r="52" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" customFormat="1">
       <c r="A52" s="23" t="s">
         <v>40</v>
       </c>
@@ -4654,7 +4695,7 @@
         <v>2566.8000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" customFormat="1">
       <c r="A53" s="23" t="s">
         <v>41</v>
       </c>
@@ -4734,7 +4775,7 @@
         <v>536234.69999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" customFormat="1">
       <c r="A54" s="23" t="s">
         <v>42</v>
       </c>
@@ -4814,7 +4855,7 @@
         <v>19647.3</v>
       </c>
     </row>
-    <row r="55" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" customFormat="1">
       <c r="A55" s="23" t="s">
         <v>43</v>
       </c>
@@ -4894,7 +4935,7 @@
         <v>32823</v>
       </c>
     </row>
-    <row r="56" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" customFormat="1">
       <c r="A56" s="23" t="s">
         <v>44</v>
       </c>
@@ -4974,7 +5015,7 @@
         <v>13175.7</v>
       </c>
     </row>
-    <row r="57" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" customFormat="1">
       <c r="A57" s="23" t="s">
         <v>45</v>
       </c>
@@ -5054,7 +5095,7 @@
         <v>555882</v>
       </c>
     </row>
-    <row r="58" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" customFormat="1">
       <c r="A58" s="23"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -5082,7 +5123,7 @@
       <c r="Y58" s="6"/>
       <c r="Z58" s="36"/>
     </row>
-    <row r="59" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" customFormat="1">
       <c r="A59" s="23" t="s">
         <v>46</v>
       </c>
@@ -5162,7 +5203,7 @@
         <v>534778.30000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" customFormat="1">
       <c r="A60" s="23" t="s">
         <v>47</v>
       </c>
@@ -5242,7 +5283,7 @@
         <v>401411</v>
       </c>
     </row>
-    <row r="61" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" customFormat="1">
       <c r="A61" s="23" t="s">
         <v>48</v>
       </c>
@@ -5322,7 +5363,7 @@
         <v>133371</v>
       </c>
     </row>
-    <row r="62" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" customFormat="1">
       <c r="A62" s="23"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -5350,7 +5391,7 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="36"/>
     </row>
-    <row r="63" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" customFormat="1">
       <c r="A63" s="23" t="s">
         <v>88</v>
       </c>
@@ -5430,7 +5471,7 @@
         <v>527035.5</v>
       </c>
     </row>
-    <row r="64" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" customFormat="1">
       <c r="A64" s="23" t="s">
         <v>89</v>
       </c>
@@ -5510,7 +5551,7 @@
         <v>287344.59999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" customFormat="1">
       <c r="A65" s="23" t="s">
         <v>90</v>
       </c>
@@ -5590,7 +5631,7 @@
         <v>92382.7</v>
       </c>
     </row>
-    <row r="66" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" customFormat="1">
       <c r="A66" s="26" t="s">
         <v>91</v>
       </c>
@@ -5670,7 +5711,7 @@
         <v>94608.9</v>
       </c>
     </row>
-    <row r="67" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" s="5" customFormat="1">
       <c r="A67" s="2" t="s">
         <v>49</v>
       </c>
@@ -5684,7 +5725,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -5697,7 +5738,7 @@
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26">
       <c r="A69" s="2" t="s">
         <v>50</v>
       </c>
@@ -5710,7 +5751,7 @@
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26">
       <c r="X70" s="5"/>
     </row>
   </sheetData>
@@ -5725,25 +5766,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="72.6640625" style="3" customWidth="1"/>
-    <col min="2" max="41" width="15.6640625" style="3" customWidth="1"/>
-    <col min="42" max="16384" width="8.6640625" style="3"/>
+    <col min="1" max="1" width="72.7109375" style="3" customWidth="1"/>
+    <col min="2" max="41" width="15.7109375" style="3" customWidth="1"/>
+    <col min="42" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="5" customFormat="1">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
         <v>51</v>
@@ -5752,7 +5793,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" customFormat="1">
       <c r="A5" s="22"/>
       <c r="B5" s="16" t="s">
         <v>2</v>
@@ -5827,7 +5868,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" customFormat="1">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -5856,7 +5897,7 @@
       <c r="X6" s="18"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" customFormat="1">
       <c r="A7" s="24"/>
       <c r="B7" s="20">
         <v>1995</v>
@@ -5931,7 +5972,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" customFormat="1">
       <c r="A8" s="25" t="s">
         <v>52</v>
       </c>
@@ -6008,7 +6049,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" customFormat="1">
       <c r="A9" s="23" t="s">
         <v>13</v>
       </c>
@@ -6085,7 +6126,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" customFormat="1">
       <c r="A10" s="23" t="s">
         <v>14</v>
       </c>
@@ -6162,7 +6203,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" customFormat="1">
       <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
@@ -6239,7 +6280,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="12" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" customFormat="1">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
@@ -6316,7 +6357,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="13" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" customFormat="1">
       <c r="A13" s="23" t="s">
         <v>17</v>
       </c>
@@ -6345,7 +6386,7 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="36"/>
     </row>
-    <row r="14" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" customFormat="1">
       <c r="A14" s="23" t="s">
         <v>18</v>
       </c>
@@ -6422,7 +6463,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" customFormat="1">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
@@ -6499,7 +6540,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" customFormat="1">
       <c r="A16" s="23" t="s">
         <v>20</v>
       </c>
@@ -6576,7 +6617,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="17" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" customFormat="1">
       <c r="A17" s="23"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -6603,7 +6644,7 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="36"/>
     </row>
-    <row r="18" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" customFormat="1">
       <c r="A18" s="23" t="s">
         <v>53</v>
       </c>
@@ -6680,7 +6721,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" customFormat="1">
       <c r="A19" s="23" t="s">
         <v>22</v>
       </c>
@@ -6709,7 +6750,7 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="36"/>
     </row>
-    <row r="20" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" customFormat="1">
       <c r="A20" s="23" t="s">
         <v>23</v>
       </c>
@@ -6786,7 +6827,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" customFormat="1">
       <c r="A21" s="23" t="s">
         <v>24</v>
       </c>
@@ -6863,7 +6904,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" customFormat="1">
       <c r="A22" s="23" t="s">
         <v>79</v>
       </c>
@@ -6940,7 +6981,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" customFormat="1">
       <c r="A23" s="23" t="s">
         <v>25</v>
       </c>
@@ -7017,7 +7058,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" customFormat="1">
       <c r="A24" s="23" t="s">
         <v>26</v>
       </c>
@@ -7094,7 +7135,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" customFormat="1">
       <c r="A25" s="23" t="s">
         <v>30</v>
       </c>
@@ -7171,7 +7212,7 @@
         <v>-4.9000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" customFormat="1">
       <c r="A26" s="23" t="s">
         <v>31</v>
       </c>
@@ -7248,7 +7289,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="27" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" customFormat="1">
       <c r="A27" s="35" t="s">
         <v>54</v>
       </c>
@@ -7325,7 +7366,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" customFormat="1">
       <c r="A28" s="35" t="s">
         <v>30</v>
       </c>
@@ -7402,7 +7443,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" customFormat="1">
       <c r="A29" s="35" t="s">
         <v>31</v>
       </c>
@@ -7479,7 +7520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" customFormat="1">
       <c r="A30" s="35" t="s">
         <v>32</v>
       </c>
@@ -7556,7 +7597,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" customFormat="1">
       <c r="A31" s="35" t="s">
         <v>95</v>
       </c>
@@ -7633,7 +7674,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" customFormat="1">
       <c r="A32" s="35" t="s">
         <v>56</v>
       </c>
@@ -7710,7 +7751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" customFormat="1">
       <c r="A33" s="35" t="s">
         <v>96</v>
       </c>
@@ -7787,7 +7828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" customFormat="1">
       <c r="A34" s="35" t="s">
         <v>97</v>
       </c>
@@ -7864,7 +7905,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" customFormat="1">
       <c r="A35" s="35" t="s">
         <v>98</v>
       </c>
@@ -7941,7 +7982,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" customFormat="1">
       <c r="A36" s="35" t="s">
         <v>99</v>
       </c>
@@ -8018,7 +8059,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" customFormat="1">
       <c r="A37" s="35" t="s">
         <v>54</v>
       </c>
@@ -8095,7 +8136,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" customFormat="1">
       <c r="A38" s="35" t="s">
         <v>33</v>
       </c>
@@ -8172,7 +8213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" customFormat="1">
       <c r="A39" s="35" t="s">
         <v>34</v>
       </c>
@@ -8249,7 +8290,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" customFormat="1">
       <c r="A40" s="23" t="s">
         <v>57</v>
       </c>
@@ -8326,7 +8367,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" customFormat="1">
       <c r="A41" s="23" t="s">
         <v>36</v>
       </c>
@@ -8403,7 +8444,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="42" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" customFormat="1">
       <c r="A42" s="23" t="s">
         <v>84</v>
       </c>
@@ -8480,7 +8521,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="43" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" customFormat="1">
       <c r="A43" s="23" t="s">
         <v>85</v>
       </c>
@@ -8557,7 +8598,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="44" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" customFormat="1">
       <c r="A44" s="23" t="s">
         <v>37</v>
       </c>
@@ -8634,7 +8675,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" customFormat="1">
       <c r="A45" s="23" t="s">
         <v>86</v>
       </c>
@@ -8711,7 +8752,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="46" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" customFormat="1">
       <c r="A46" s="23" t="s">
         <v>87</v>
       </c>
@@ -8788,7 +8829,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" customFormat="1">
       <c r="A47" s="23" t="s">
         <v>38</v>
       </c>
@@ -8817,7 +8858,7 @@
       <c r="X47" s="6"/>
       <c r="Y47" s="36"/>
     </row>
-    <row r="48" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" customFormat="1">
       <c r="A48" s="23" t="s">
         <v>72</v>
       </c>
@@ -8894,7 +8935,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="49" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" customFormat="1">
       <c r="A49" s="23"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -8921,7 +8962,7 @@
       <c r="X49" s="6"/>
       <c r="Y49" s="36"/>
     </row>
-    <row r="50" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" customFormat="1">
       <c r="A50" s="23" t="s">
         <v>40</v>
       </c>
@@ -8998,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" customFormat="1">
       <c r="A51" s="23" t="s">
         <v>41</v>
       </c>
@@ -9075,7 +9116,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" customFormat="1">
       <c r="A52" s="23" t="s">
         <v>42</v>
       </c>
@@ -9152,7 +9193,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" customFormat="1">
       <c r="A53" s="23" t="s">
         <v>43</v>
       </c>
@@ -9229,7 +9270,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="54" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" customFormat="1">
       <c r="A54" s="23" t="s">
         <v>44</v>
       </c>
@@ -9306,7 +9347,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="55" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" customFormat="1">
       <c r="A55" s="23" t="s">
         <v>45</v>
       </c>
@@ -9383,7 +9424,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="56" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" customFormat="1">
       <c r="A56" s="23"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -9410,7 +9451,7 @@
       <c r="X56" s="6"/>
       <c r="Y56" s="36"/>
     </row>
-    <row r="57" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" customFormat="1">
       <c r="A57" s="23" t="s">
         <v>46</v>
       </c>
@@ -9487,7 +9528,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="58" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" customFormat="1">
       <c r="A58" s="23" t="s">
         <v>47</v>
       </c>
@@ -9564,7 +9605,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" customFormat="1">
       <c r="A59" s="23" t="s">
         <v>48</v>
       </c>
@@ -9641,7 +9682,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="60" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" customFormat="1">
       <c r="A60" s="23"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -9668,7 +9709,7 @@
       <c r="X60" s="6"/>
       <c r="Y60" s="36"/>
     </row>
-    <row r="61" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" customFormat="1">
       <c r="A61" s="23" t="s">
         <v>88</v>
       </c>
@@ -9745,7 +9786,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="62" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" customFormat="1">
       <c r="A62" s="23" t="s">
         <v>89</v>
       </c>
@@ -9822,7 +9863,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="63" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" customFormat="1">
       <c r="A63" s="23" t="s">
         <v>90</v>
       </c>
@@ -9899,7 +9940,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="64" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" customFormat="1">
       <c r="A64" s="26" t="s">
         <v>91</v>
       </c>
@@ -9976,7 +10017,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" s="5" customFormat="1">
       <c r="A65" s="2" t="s">
         <v>76</v>
       </c>
@@ -9984,14 +10025,14 @@
       <c r="C65" s="8"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>38</v>
       </c>
@@ -10010,25 +10051,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" style="9" customWidth="1"/>
-    <col min="2" max="41" width="15.6640625" style="9" customWidth="1"/>
-    <col min="42" max="16384" width="8.6640625" style="9"/>
+    <col min="1" max="1" width="52.7109375" style="9" customWidth="1"/>
+    <col min="2" max="41" width="15.7109375" style="9" customWidth="1"/>
+    <col min="42" max="16384" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="11" customFormat="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>58</v>
@@ -10038,7 +10079,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" customFormat="1">
       <c r="A5" s="27"/>
       <c r="B5" s="16" t="s">
         <v>2</v>
@@ -10113,7 +10154,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" customFormat="1">
       <c r="A6" s="28" t="s">
         <v>11</v>
       </c>
@@ -10142,7 +10183,7 @@
       <c r="X6" s="18"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" customFormat="1">
       <c r="A7" s="29"/>
       <c r="B7" s="20">
         <v>1995</v>
@@ -10217,7 +10258,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" customFormat="1">
       <c r="A8" s="30" t="s">
         <v>59</v>
       </c>
@@ -10294,7 +10335,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" customFormat="1">
       <c r="A9" s="31" t="s">
         <v>60</v>
       </c>
@@ -10371,7 +10412,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" customFormat="1">
       <c r="A10" s="31" t="s">
         <v>61</v>
       </c>
@@ -10448,7 +10489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" customFormat="1">
       <c r="A11" s="31" t="s">
         <v>62</v>
       </c>
@@ -10525,7 +10566,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" customFormat="1">
       <c r="A12" s="31" t="s">
         <v>63</v>
       </c>
@@ -10602,7 +10643,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" customFormat="1">
       <c r="A13" s="31" t="s">
         <v>100</v>
       </c>
@@ -10679,7 +10720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" customFormat="1">
       <c r="A14" s="31" t="s">
         <v>64</v>
       </c>
@@ -10756,7 +10797,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" customFormat="1">
       <c r="A15" s="31" t="s">
         <v>65</v>
       </c>
@@ -10833,7 +10874,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" customFormat="1">
       <c r="A16" s="31" t="s">
         <v>66</v>
       </c>
@@ -10910,7 +10951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" customFormat="1">
       <c r="A17" s="31" t="s">
         <v>101</v>
       </c>
@@ -10987,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" customFormat="1">
       <c r="A18" s="32" t="s">
         <v>67</v>
       </c>
@@ -11064,7 +11105,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" customFormat="1">
       <c r="A19" s="32" t="s">
         <v>68</v>
       </c>
@@ -11141,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" customFormat="1">
       <c r="A20" s="31" t="s">
         <v>69</v>
       </c>
@@ -11218,7 +11259,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" customFormat="1">
       <c r="A21" s="31" t="s">
         <v>36</v>
       </c>
@@ -11295,7 +11336,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" customFormat="1">
       <c r="A22" s="31" t="s">
         <v>37</v>
       </c>
@@ -11372,7 +11413,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" customFormat="1">
       <c r="A23" s="32"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -11399,7 +11440,7 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="36"/>
     </row>
-    <row r="24" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" customFormat="1">
       <c r="A24" s="33" t="s">
         <v>74</v>
       </c>
@@ -11476,7 +11517,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" s="11" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>107</v>
       </c>
@@ -11486,7 +11527,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25">
       <c r="A26" s="9" t="s">
         <v>70</v>
       </c>
@@ -11496,7 +11537,7 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25">
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>

</xml_diff>